<commit_message>
slider automatically scrolling purpose
slider automatically scrolling purpose
</commit_message>
<xml_diff>
--- a/uploads/Electroniccategoryfilemobiles.xlsx
+++ b/uploads/Electroniccategoryfilemobiles.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
   <si>
     <t>sno</t>
   </si>
@@ -148,12 +148,6 @@
   </si>
   <si>
     <t>Product image12</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>10</t>
   </si>
   <si>
     <t>subitem</t>
@@ -592,7 +586,7 @@
   <dimension ref="A1:AT2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -661,10 +655,10 @@
         <v>31</v>
       </c>
       <c r="O1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>24</v>
@@ -673,52 +667,52 @@
         <v>25</v>
       </c>
       <c r="S1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="T1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="V1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="Y1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AE1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="AG1" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="AH1" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AI1" s="2" t="s">
         <v>32</v>
@@ -762,10 +756,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>18</v>
@@ -776,12 +770,6 @@
       <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="I2" s="1" t="s">
         <v>20</v>
       </c>
@@ -798,13 +786,13 @@
         <v>23</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="Q2" t="s">
         <v>26</v>
@@ -813,52 +801,52 @@
         <v>27</v>
       </c>
       <c r="S2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="W2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AD2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AF2" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="AG2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="AI2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
products impoart file  purpose
products impoart file  purpose
</commit_message>
<xml_diff>
--- a/uploads/Electroniccategoryfilemobiles.xlsx
+++ b/uploads/Electroniccategoryfilemobiles.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
   <si>
     <t>sno</t>
   </si>
@@ -75,18 +75,9 @@
     <t>otherunique</t>
   </si>
   <si>
-    <t>999</t>
-  </si>
-  <si>
     <t>50</t>
   </si>
   <si>
-    <t>metakeyword</t>
-  </si>
-  <si>
-    <t>meta tile</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -102,9 +93,6 @@
     <t>4gb,500gb</t>
   </si>
   <si>
-    <t>55555</t>
-  </si>
-  <si>
     <t>Offers</t>
   </si>
   <si>
@@ -156,36 +144,21 @@
     <t>Brand</t>
   </si>
   <si>
-    <t>puma</t>
-  </si>
-  <si>
     <t>Ideal for</t>
   </si>
   <si>
-    <t>ideal for</t>
-  </si>
-  <si>
     <t>Screen size</t>
   </si>
   <si>
     <t>Operating System</t>
   </si>
   <si>
-    <t>os</t>
-  </si>
-  <si>
     <t>Ram</t>
   </si>
   <si>
-    <t>4gb</t>
-  </si>
-  <si>
     <t>Internal storage</t>
   </si>
   <si>
-    <t>internal Storage</t>
-  </si>
-  <si>
     <t>Network type</t>
   </si>
   <si>
@@ -198,9 +171,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>Operating system version name</t>
   </si>
   <si>
@@ -219,22 +189,25 @@
     <t>Sim Type</t>
   </si>
   <si>
-    <t>sim type</t>
-  </si>
-  <si>
     <t>Clock Speed</t>
   </si>
   <si>
     <t>No.of Cores</t>
   </si>
   <si>
-    <t>no.of cores</t>
-  </si>
-  <si>
     <t>mobiles</t>
   </si>
   <si>
     <t>sony</t>
+  </si>
+  <si>
+    <t>23000</t>
+  </si>
+  <si>
+    <t>Sony</t>
+  </si>
+  <si>
+    <t>22000</t>
   </si>
 </sst>
 </file>
@@ -586,7 +559,7 @@
   <dimension ref="A1:AT2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -631,10 +604,10 @@
         <v>13</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>14</v>
@@ -652,103 +625,103 @@
         <v>17</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:46">
@@ -756,98 +729,57 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>26</v>
-      </c>
       <c r="R2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
       <c r="AI2" t="s">
         <v>3</v>
       </c>

</xml_diff>